<commit_message>
updated without service account till date.
</commit_message>
<xml_diff>
--- a/calls.xlsx
+++ b/calls.xlsx
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>https://cloudphone.tatateleservices.com/file/recording?callId=1752055968.539653&amp;type=rec&amp;token=YWNZSnlOSnhuVzBtYnR0ek1xZlpnK25nMDgzZENlejhKdFA2cEoxYndlNHpYNWEySnZrZEtNS28zZjRUc25kUDo6YWIxMjM0Y2Q1NnJ0eXl1dQ%3D%3D</t>
+  </si>
+  <si>
+    <t>recording_url</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15"/>
@@ -480,59 +483,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
@@ -550,18 +533,28 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="s">
-        <v>27</v>
+      <c r="A11" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="s">
-        <v>28</v>
+      <c r="A12" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="9" t="s">
-        <v>29</v>
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>